<commit_message>
Modified create_chart(), created make_chart(), chart_legend(), chart_title() functions
</commit_message>
<xml_diff>
--- a/LumenConfig.xlsx
+++ b/LumenConfig.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cathy Hsu\Light and Motion\data_processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B70D8C86-DE72-4EAF-BB8F-CA2ED35F4F87}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD214791-36BE-444C-AD68-3995ECBAF5F9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E72AF285-2932-4A33-BA96-70EF447B094A}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Format</t>
   </si>
@@ -49,9 +49,6 @@
     <t>AB</t>
   </si>
   <si>
-    <t>F</t>
-  </si>
-  <si>
     <t>I</t>
   </si>
   <si>
@@ -61,9 +58,6 @@
     <t>B</t>
   </si>
   <si>
-    <t>E</t>
-  </si>
-  <si>
     <t>Title</t>
   </si>
   <si>
@@ -89,6 +83,18 @@
   </si>
   <si>
     <t xml:space="preserve">Hello </t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
   </si>
 </sst>
 </file>
@@ -443,7 +449,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -467,15 +473,15 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -484,7 +490,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -492,27 +498,27 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -520,18 +526,15 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
@@ -539,8 +542,11 @@
       <c r="C6">
         <v>1</v>
       </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated time_format() code to store datetime objects in Date/Time column
</commit_message>
<xml_diff>
--- a/LumenConfig.xlsx
+++ b/LumenConfig.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cathy Hsu\Light and Motion\data_processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD214791-36BE-444C-AD68-3995ECBAF5F9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82AF697B-7D77-4C30-8D6F-0E6737D16339}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E72AF285-2932-4A33-BA96-70EF447B094A}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Format</t>
   </si>
@@ -67,18 +67,12 @@
     <t>Color Rendering (R4)</t>
   </si>
   <si>
-    <t>Radiant Flux (Watts)</t>
-  </si>
-  <si>
     <t>Luminous Flux (lumens)</t>
   </si>
   <si>
     <t>Graph Title</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -95,6 +89,9 @@
   </si>
   <si>
     <t>f</t>
+  </si>
+  <si>
+    <t>radiant flux (Watts)</t>
   </si>
 </sst>
 </file>
@@ -449,7 +446,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -476,12 +473,12 @@
         <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -490,7 +487,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -498,10 +495,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
         <v>12</v>
@@ -509,16 +503,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -528,8 +522,11 @@
       <c r="B5" t="s">
         <v>8</v>
       </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -543,7 +540,7 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Added range functionality to configuration file
</commit_message>
<xml_diff>
--- a/LumenConfig.xlsx
+++ b/LumenConfig.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cathy Hsu\Light and Motion\data_processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7C07A2-7996-495A-BD70-2CC8B0F592BE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C5CFD1-F65A-4D53-BFA3-777FBD814893}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E72AF285-2932-4A33-BA96-70EF447B094A}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>Format</t>
   </si>
@@ -92,6 +92,36 @@
   </si>
   <si>
     <t>Scan</t>
+  </si>
+  <si>
+    <t>Header</t>
+  </si>
+  <si>
+    <t>X Min</t>
+  </si>
+  <si>
+    <t>X Max</t>
+  </si>
+  <si>
+    <t>Y Min</t>
+  </si>
+  <si>
+    <t>Y Max</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>9:20</t>
+  </si>
+  <si>
+    <t>2:5</t>
+  </si>
+  <si>
+    <t>3:6</t>
+  </si>
+  <si>
+    <t>1:4</t>
   </si>
 </sst>
 </file>
@@ -127,8 +157,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6FDB1BB-D33E-4BA3-BD32-0B8598E9403D}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -456,7 +487,7 @@
     <col min="6" max="6" width="15.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -475,8 +506,11 @@
       <c r="F1" t="s">
         <v>14</v>
       </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -489,8 +523,11 @@
       <c r="E2" t="s">
         <v>21</v>
       </c>
+      <c r="G2" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -500,8 +537,11 @@
       <c r="E3" t="s">
         <v>12</v>
       </c>
+      <c r="G3" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -514,8 +554,11 @@
       <c r="E4" t="s">
         <v>20</v>
       </c>
+      <c r="G4" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -528,8 +571,9 @@
       <c r="E5" t="s">
         <v>13</v>
       </c>
+      <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -544,21 +588,45 @@
       </c>
       <c r="E6" t="s">
         <v>11</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA76AB39-CB93-43F9-8C95-F36AEC9A6A90}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed empty string issue
</commit_message>
<xml_diff>
--- a/LumenConfig.xlsx
+++ b/LumenConfig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cathy Hsu\Light and Motion\data_processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{127C90F0-E104-4267-AAAC-504BAF5339AB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244E4304-BCA8-4694-8D9A-81BF6FDC36E7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{E72AF285-2932-4A33-BA96-70EF447B094A}"/>
+    <workbookView xWindow="2530" yWindow="300" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{E72AF285-2932-4A33-BA96-70EF447B094A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>Format</t>
   </si>
@@ -76,9 +76,6 @@
     <t>y</t>
   </si>
   <si>
-    <t>e</t>
-  </si>
-  <si>
     <t>f</t>
   </si>
   <si>
@@ -112,9 +109,6 @@
     <t>Time Unit</t>
   </si>
   <si>
-    <t>Time Axis</t>
-  </si>
-  <si>
     <t>Grid Lines</t>
   </si>
   <si>
@@ -137,9 +131,6 @@
   </si>
   <si>
     <t>Chromatic</t>
-  </si>
-  <si>
-    <t>4:10</t>
   </si>
   <si>
     <t>Yes</t>
@@ -495,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6FDB1BB-D33E-4BA3-BD32-0B8598E9403D}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -508,7 +499,7 @@
     <col min="6" max="6" width="15.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -519,57 +510,66 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>13</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
@@ -577,17 +577,14 @@
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -595,13 +592,16 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>33</v>
+      <c r="G6" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -612,53 +612,47 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA76AB39-CB93-43F9-8C95-F36AEC9A6A90}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="H1" sqref="H1:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" t="s">
-        <v>22</v>
-      </c>
       <c r="G1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" t="s">
         <v>29</v>
-      </c>
-      <c r="H1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" t="s">
-        <v>28</v>
       </c>
       <c r="J1" t="s">
         <v>30</v>
       </c>
-      <c r="K1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B2">
         <v>2</v>
       </c>
@@ -668,14 +662,8 @@
       <c r="F2">
         <v>1000</v>
       </c>
-      <c r="H2" t="s">
-        <v>5</v>
-      </c>
       <c r="I2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added pdf output functionality
</commit_message>
<xml_diff>
--- a/LumenConfig.xlsx
+++ b/LumenConfig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cathy Hsu\Light and Motion\data_processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244E4304-BCA8-4694-8D9A-81BF6FDC36E7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BABF24D-0273-4678-9956-96798A44EEF7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2530" yWindow="300" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{E72AF285-2932-4A33-BA96-70EF447B094A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{E72AF285-2932-4A33-BA96-70EF447B094A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>Format</t>
   </si>
@@ -49,12 +49,6 @@
     <t>AB</t>
   </si>
   <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
@@ -76,9 +70,6 @@
     <t>y</t>
   </si>
   <si>
-    <t>f</t>
-  </si>
-  <si>
     <t>Scan</t>
   </si>
   <si>
@@ -134,6 +125,9 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>E</t>
   </si>
 </sst>
 </file>
@@ -489,7 +483,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -510,30 +504,30 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -541,13 +535,13 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -555,53 +549,53 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -622,34 +616,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" t="s">
         <v>27</v>
-      </c>
-      <c r="H1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
@@ -663,7 +657,7 @@
         <v>1000</v>
       </c>
       <c r="I2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Debugged default options for 'General Settings'
</commit_message>
<xml_diff>
--- a/LumenConfig.xlsx
+++ b/LumenConfig.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cathy Hsu\Light and Motion\data_processing\error_fixing\data_processing-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cathy Hsu\Light and Motion\data_processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E83779FE-9FB4-4ECA-AE45-1ADFBA61A6A2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C472616-B388-4AEE-8C86-2BFB559F0963}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4700" yWindow="1200" windowWidth="14160" windowHeight="7370" activeTab="1" xr2:uid="{E72AF285-2932-4A33-BA96-70EF447B094A}"/>
+    <workbookView xWindow="1480" yWindow="1480" windowWidth="14160" windowHeight="7370" activeTab="1" xr2:uid="{E72AF285-2932-4A33-BA96-70EF447B094A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
   <si>
     <t>Format</t>
   </si>
@@ -146,9 +146,6 @@
   </si>
   <si>
     <t>Time Unit</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -633,7 +630,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -683,15 +680,6 @@
       <c r="B2">
         <v>2</v>
       </c>
-      <c r="C2">
-        <v>41</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="M2" t="s">
-        <v>40</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added functionality for generating a txt file
</commit_message>
<xml_diff>
--- a/LumenConfig.xlsx
+++ b/LumenConfig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cathy Hsu\Light and Motion\data_processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C472616-B388-4AEE-8C86-2BFB559F0963}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB37FEC-998C-426C-BCDB-96B941362A75}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="1480" windowWidth="14160" windowHeight="7370" activeTab="1" xr2:uid="{E72AF285-2932-4A33-BA96-70EF447B094A}"/>
+    <workbookView xWindow="4330" yWindow="610" windowWidth="14160" windowHeight="7370" activeTab="1" xr2:uid="{E72AF285-2932-4A33-BA96-70EF447B094A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t>Format</t>
   </si>
@@ -146,6 +146,15 @@
   </si>
   <si>
     <t>Time Unit</t>
+  </si>
+  <si>
+    <t>TXT</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -627,15 +636,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA76AB39-CB93-43F9-8C95-F36AEC9A6A90}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -673,12 +682,27 @@
         <v>34</v>
       </c>
       <c r="M1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B2">
         <v>2</v>
+      </c>
+      <c r="C2">
+        <v>41</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="L2" t="s">
+        <v>41</v>
+      </c>
+      <c r="N2" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moved legend outside of plot area
</commit_message>
<xml_diff>
--- a/LumenConfig.xlsx
+++ b/LumenConfig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cathy Hsu\Light and Motion\data_processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D2DCFE-D885-45D9-9C32-335F65263E92}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B993C8-D22F-4D98-A959-40753BEDB4B0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E72AF285-2932-4A33-BA96-70EF447B094A}"/>
+    <workbookView xWindow="1820" yWindow="1820" windowWidth="14160" windowHeight="7700" activeTab="1" xr2:uid="{E72AF285-2932-4A33-BA96-70EF447B094A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>Format</t>
   </si>
@@ -34,112 +34,91 @@
     <t>Axis</t>
   </si>
   <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>X Min</t>
+  </si>
+  <si>
+    <t>X Max</t>
+  </si>
+  <si>
+    <t>Y Min</t>
+  </si>
+  <si>
+    <t>Y Max</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>Start Row</t>
+  </si>
+  <si>
+    <t>Chart Title</t>
+  </si>
+  <si>
+    <t>Grid Lines</t>
+  </si>
+  <si>
+    <t>Excel</t>
+  </si>
+  <si>
+    <t>JPEG</t>
+  </si>
+  <si>
+    <t>PDF</t>
+  </si>
+  <si>
+    <t>Stop Row</t>
+  </si>
+  <si>
+    <t>Transpose</t>
+  </si>
+  <si>
+    <t>Time Unit</t>
+  </si>
+  <si>
+    <t>TXT</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>4:</t>
+  </si>
+  <si>
+    <t>Elapsed Time</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
     <t>C</t>
   </si>
   <si>
-    <t>Input</t>
-  </si>
-  <si>
-    <t>Output</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>AB</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Graph Title</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>X Min</t>
-  </si>
-  <si>
-    <t>X Max</t>
-  </si>
-  <si>
-    <t>Y Min</t>
-  </si>
-  <si>
-    <t>Y Max</t>
-  </si>
-  <si>
-    <t>Range</t>
-  </si>
-  <si>
-    <t>9:20</t>
-  </si>
-  <si>
-    <t>2:5</t>
-  </si>
-  <si>
-    <t>Start Row</t>
-  </si>
-  <si>
-    <t>Chart Title</t>
-  </si>
-  <si>
-    <t>Grid Lines</t>
-  </si>
-  <si>
-    <t>Excel</t>
-  </si>
-  <si>
-    <t>JPEG</t>
-  </si>
-  <si>
-    <t>PDF</t>
-  </si>
-  <si>
-    <t>Stop Row</t>
-  </si>
-  <si>
-    <t>Skip Row</t>
-  </si>
-  <si>
-    <t>Transpose</t>
-  </si>
-  <si>
-    <t>5:20</t>
-  </si>
-  <si>
-    <t>Time Unit</t>
-  </si>
-  <si>
-    <t>TXT</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>H</t>
   </si>
 </sst>
 </file>
@@ -492,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6FDB1BB-D33E-4BA3-BD32-0B8598E9403D}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -505,98 +484,82 @@
     <col min="6" max="6" width="15.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4">
         <v>2</v>
       </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="G4" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -606,73 +569,70 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA76AB39-CB93-43F9-8C95-F36AEC9A6A90}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="L1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" t="s">
         <v>19</v>
       </c>
-      <c r="H1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B2">
         <v>2</v>
       </c>
       <c r="C2">
-        <v>41</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="L2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N2" t="s">
-        <v>37</v>
+        <v>22</v>
+      </c>
+      <c r="F2">
+        <v>0.1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>